<commit_message>
edit docker-compose.yaml password to password
</commit_message>
<xml_diff>
--- a/public/uploads/attendance_data_001001.xlsx
+++ b/public/uploads/attendance_data_001001.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -406,6 +406,7 @@
     <col min="2" max="2" width="14.83203125" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -421,6 +422,9 @@
       <c r="D1" t="str">
         <v>01/01/2555</v>
       </c>
+      <c r="E1" t="str">
+        <v>02/01/2555</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -435,6 +439,9 @@
       <c r="D2" t="str">
         <v>มาเรียน</v>
       </c>
+      <c r="E2" t="str">
+        <v>ขาดเรียน</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -449,10 +456,13 @@
       <c r="D3" t="str">
         <v>มาเรียน</v>
       </c>
+      <c r="E3" t="str">
+        <v>มาเรียน</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
edit export file to add description after the date and add get attendance
</commit_message>
<xml_diff>
--- a/public/uploads/attendance_data_001001.xlsx
+++ b/public/uploads/attendance_data_001001.xlsx
@@ -397,16 +397,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -420,27 +419,21 @@
         <v>อีเมล</v>
       </c>
       <c r="D1" t="str">
-        <v>01/01/2555</v>
-      </c>
-      <c r="E1" t="str">
-        <v>02/01/2555</v>
+        <v>2025-02-23 - HW1</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>650610700</v>
+        <v>650610759</v>
       </c>
       <c r="B2" t="str">
-        <v>kun</v>
+        <v>earn</v>
       </c>
       <c r="C2" t="str">
-        <v>kun@gamil.com</v>
+        <v>earn@example.com</v>
       </c>
       <c r="D2" t="str">
         <v>มาเรียน</v>
-      </c>
-      <c r="E2" t="str">
-        <v>ขาดเรียน</v>
       </c>
     </row>
     <row r="3">
@@ -454,15 +447,12 @@
         <v>hi@gamil.com</v>
       </c>
       <c r="D3" t="str">
-        <v>มาเรียน</v>
-      </c>
-      <c r="E3" t="str">
-        <v>มาเรียน</v>
+        <v>ขาดเรียน</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>